<commit_message>
added 06-07season and added error bars to plots
</commit_message>
<xml_diff>
--- a/NHL_stats.xlsx
+++ b/NHL_stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kyle\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ktdav\Downloads\CMSE202\repositories\CMSE202_Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516AB577-A967-4A40-AF98-B2A33E2F3C40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09AFF9B0-E259-4DC4-92AD-5D1F9BF2D26E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="10" xr2:uid="{452875C4-1392-4CAE-81A4-BEC72B79344C}"/>
+    <workbookView xWindow="3045" yWindow="2827" windowWidth="14400" windowHeight="7373" activeTab="11" xr2:uid="{452875C4-1392-4CAE-81A4-BEC72B79344C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,8 +24,9 @@
     <sheet name="Sheet9" sheetId="9" r:id="rId9"/>
     <sheet name="Sheet10" sheetId="10" r:id="rId10"/>
     <sheet name="Sheet11" sheetId="11" r:id="rId11"/>
+    <sheet name="Sheet12" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,9 +34,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -43,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="110">
   <si>
     <t>Special Teams</t>
   </si>
@@ -368,12 +367,18 @@
   <si>
     <t>2007-2008</t>
   </si>
+  <si>
+    <t>Atlanta Thrashers*</t>
+  </si>
+  <si>
+    <t>2006-2007</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -383,6 +388,11 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="5"/>
       <color rgb="FF000000"/>
       <name val="Arial Unicode MS"/>
     </font>
@@ -407,9 +417,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -732,7 +745,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:33">
       <c r="A1" s="1"/>
@@ -4112,7 +4125,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:33">
       <c r="A1" s="1"/>
@@ -7386,11 +7399,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7A7F241-0B91-47B0-985B-15D2C634661E}">
   <dimension ref="A1:AG33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:33">
       <c r="A1" s="1"/>
@@ -10657,6 +10670,3285 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6195787-E514-4BF1-8594-6D9AF7CB68DE}">
+  <dimension ref="A1:AG33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="1" spans="1:33">
+      <c r="A1" s="2"/>
+      <c r="S1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V1" t="s">
+        <v>0</v>
+      </c>
+      <c r="W1" t="s">
+        <v>0</v>
+      </c>
+      <c r="X1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R2" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" t="s">
+        <v>19</v>
+      </c>
+      <c r="T2" t="s">
+        <v>20</v>
+      </c>
+      <c r="U2" t="s">
+        <v>21</v>
+      </c>
+      <c r="V2" t="s">
+        <v>22</v>
+      </c>
+      <c r="W2" t="s">
+        <v>23</v>
+      </c>
+      <c r="X2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3">
+        <v>27.2</v>
+      </c>
+      <c r="D3">
+        <v>82</v>
+      </c>
+      <c r="E3">
+        <v>53</v>
+      </c>
+      <c r="F3">
+        <v>22</v>
+      </c>
+      <c r="G3">
+        <v>7</v>
+      </c>
+      <c r="H3">
+        <v>113</v>
+      </c>
+      <c r="I3">
+        <v>0.68899999999999995</v>
+      </c>
+      <c r="J3">
+        <v>298</v>
+      </c>
+      <c r="K3">
+        <v>238</v>
+      </c>
+      <c r="L3">
+        <v>10</v>
+      </c>
+      <c r="M3">
+        <v>4</v>
+      </c>
+      <c r="N3">
+        <v>0.64</v>
+      </c>
+      <c r="O3">
+        <v>-0.16</v>
+      </c>
+      <c r="P3">
+        <v>6.54</v>
+      </c>
+      <c r="Q3">
+        <v>219</v>
+      </c>
+      <c r="R3">
+        <v>153</v>
+      </c>
+      <c r="S3">
+        <v>71</v>
+      </c>
+      <c r="T3">
+        <v>407</v>
+      </c>
+      <c r="U3">
+        <v>17.440000000000001</v>
+      </c>
+      <c r="V3">
+        <v>72</v>
+      </c>
+      <c r="W3">
+        <v>386</v>
+      </c>
+      <c r="X3">
+        <v>81.349999999999994</v>
+      </c>
+      <c r="Y3">
+        <v>8</v>
+      </c>
+      <c r="Z3">
+        <v>13</v>
+      </c>
+      <c r="AA3">
+        <v>14.6</v>
+      </c>
+      <c r="AB3">
+        <v>15.2</v>
+      </c>
+      <c r="AC3">
+        <v>2417</v>
+      </c>
+      <c r="AD3">
+        <v>12.3</v>
+      </c>
+      <c r="AE3">
+        <v>2541</v>
+      </c>
+      <c r="AF3">
+        <v>0.90600000000000003</v>
+      </c>
+      <c r="AG3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="D4">
+        <v>82</v>
+      </c>
+      <c r="E4">
+        <v>50</v>
+      </c>
+      <c r="F4">
+        <v>19</v>
+      </c>
+      <c r="G4">
+        <v>13</v>
+      </c>
+      <c r="H4">
+        <v>113</v>
+      </c>
+      <c r="I4">
+        <v>0.68899999999999995</v>
+      </c>
+      <c r="J4">
+        <v>252</v>
+      </c>
+      <c r="K4">
+        <v>191</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+      <c r="M4">
+        <v>8</v>
+      </c>
+      <c r="N4">
+        <v>0.72</v>
+      </c>
+      <c r="O4">
+        <v>0.05</v>
+      </c>
+      <c r="P4">
+        <v>5.4</v>
+      </c>
+      <c r="Q4">
+        <v>172</v>
+      </c>
+      <c r="R4">
+        <v>117</v>
+      </c>
+      <c r="S4">
+        <v>68</v>
+      </c>
+      <c r="T4">
+        <v>401</v>
+      </c>
+      <c r="U4">
+        <v>16.96</v>
+      </c>
+      <c r="V4">
+        <v>63</v>
+      </c>
+      <c r="W4">
+        <v>408</v>
+      </c>
+      <c r="X4">
+        <v>84.56</v>
+      </c>
+      <c r="Y4">
+        <v>12</v>
+      </c>
+      <c r="Z4">
+        <v>11</v>
+      </c>
+      <c r="AA4">
+        <v>12</v>
+      </c>
+      <c r="AB4">
+        <v>12.4</v>
+      </c>
+      <c r="AC4">
+        <v>2771</v>
+      </c>
+      <c r="AD4">
+        <v>9.1</v>
+      </c>
+      <c r="AE4">
+        <v>2020</v>
+      </c>
+      <c r="AF4">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="AG4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5">
+        <v>28.5</v>
+      </c>
+      <c r="D5">
+        <v>82</v>
+      </c>
+      <c r="E5">
+        <v>48</v>
+      </c>
+      <c r="F5">
+        <v>20</v>
+      </c>
+      <c r="G5">
+        <v>14</v>
+      </c>
+      <c r="H5">
+        <v>110</v>
+      </c>
+      <c r="I5">
+        <v>0.67100000000000004</v>
+      </c>
+      <c r="J5">
+        <v>254</v>
+      </c>
+      <c r="K5">
+        <v>198</v>
+      </c>
+      <c r="L5">
+        <v>4</v>
+      </c>
+      <c r="M5">
+        <v>10</v>
+      </c>
+      <c r="N5">
+        <v>0.67</v>
+      </c>
+      <c r="O5">
+        <v>0.06</v>
+      </c>
+      <c r="P5">
+        <v>5.51</v>
+      </c>
+      <c r="Q5">
+        <v>161</v>
+      </c>
+      <c r="R5">
+        <v>133</v>
+      </c>
+      <c r="S5">
+        <v>89</v>
+      </c>
+      <c r="T5">
+        <v>398</v>
+      </c>
+      <c r="U5">
+        <v>22.36</v>
+      </c>
+      <c r="V5">
+        <v>61</v>
+      </c>
+      <c r="W5">
+        <v>410</v>
+      </c>
+      <c r="X5">
+        <v>85.12</v>
+      </c>
+      <c r="Y5">
+        <v>4</v>
+      </c>
+      <c r="Z5">
+        <v>4</v>
+      </c>
+      <c r="AA5">
+        <v>17.8</v>
+      </c>
+      <c r="AB5">
+        <v>17.8</v>
+      </c>
+      <c r="AC5">
+        <v>2582</v>
+      </c>
+      <c r="AD5">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="AE5">
+        <v>2248</v>
+      </c>
+      <c r="AF5">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="AG5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6">
+        <v>27.4</v>
+      </c>
+      <c r="D6">
+        <v>82</v>
+      </c>
+      <c r="E6">
+        <v>51</v>
+      </c>
+      <c r="F6">
+        <v>23</v>
+      </c>
+      <c r="G6">
+        <v>8</v>
+      </c>
+      <c r="H6">
+        <v>110</v>
+      </c>
+      <c r="I6">
+        <v>0.67100000000000004</v>
+      </c>
+      <c r="J6">
+        <v>266</v>
+      </c>
+      <c r="K6">
+        <v>207</v>
+      </c>
+      <c r="L6">
+        <v>6</v>
+      </c>
+      <c r="M6">
+        <v>5</v>
+      </c>
+      <c r="N6">
+        <v>0.78</v>
+      </c>
+      <c r="O6">
+        <v>0.05</v>
+      </c>
+      <c r="P6">
+        <v>5.77</v>
+      </c>
+      <c r="Q6">
+        <v>187</v>
+      </c>
+      <c r="R6">
+        <v>150</v>
+      </c>
+      <c r="S6">
+        <v>71</v>
+      </c>
+      <c r="T6">
+        <v>408</v>
+      </c>
+      <c r="U6">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="V6">
+        <v>55</v>
+      </c>
+      <c r="W6">
+        <v>390</v>
+      </c>
+      <c r="X6">
+        <v>85.9</v>
+      </c>
+      <c r="Y6">
+        <v>8</v>
+      </c>
+      <c r="Z6">
+        <v>2</v>
+      </c>
+      <c r="AA6">
+        <v>14.4</v>
+      </c>
+      <c r="AB6">
+        <v>15.7</v>
+      </c>
+      <c r="AC6">
+        <v>2261</v>
+      </c>
+      <c r="AD6">
+        <v>11.8</v>
+      </c>
+      <c r="AE6">
+        <v>2561</v>
+      </c>
+      <c r="AF6">
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="AG6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7">
+        <v>29.4</v>
+      </c>
+      <c r="D7">
+        <v>82</v>
+      </c>
+      <c r="E7">
+        <v>49</v>
+      </c>
+      <c r="F7">
+        <v>24</v>
+      </c>
+      <c r="G7">
+        <v>9</v>
+      </c>
+      <c r="H7">
+        <v>107</v>
+      </c>
+      <c r="I7">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="J7">
+        <v>206</v>
+      </c>
+      <c r="K7">
+        <v>193</v>
+      </c>
+      <c r="L7">
+        <v>10</v>
+      </c>
+      <c r="M7">
+        <v>8</v>
+      </c>
+      <c r="N7">
+        <v>0.03</v>
+      </c>
+      <c r="O7">
+        <v>-0.15</v>
+      </c>
+      <c r="P7">
+        <v>4.87</v>
+      </c>
+      <c r="Q7">
+        <v>137</v>
+      </c>
+      <c r="R7">
+        <v>142</v>
+      </c>
+      <c r="S7">
+        <v>65</v>
+      </c>
+      <c r="T7">
+        <v>367</v>
+      </c>
+      <c r="U7">
+        <v>17.71</v>
+      </c>
+      <c r="V7">
+        <v>40</v>
+      </c>
+      <c r="W7">
+        <v>271</v>
+      </c>
+      <c r="X7">
+        <v>85.24</v>
+      </c>
+      <c r="Y7">
+        <v>4</v>
+      </c>
+      <c r="Z7">
+        <v>11</v>
+      </c>
+      <c r="AA7">
+        <v>10.1</v>
+      </c>
+      <c r="AB7">
+        <v>12.3</v>
+      </c>
+      <c r="AC7">
+        <v>2354</v>
+      </c>
+      <c r="AD7">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="AE7">
+        <v>2332</v>
+      </c>
+      <c r="AF7">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="AG7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8">
+        <v>26.4</v>
+      </c>
+      <c r="D8">
+        <v>82</v>
+      </c>
+      <c r="E8">
+        <v>51</v>
+      </c>
+      <c r="F8">
+        <v>26</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="H8">
+        <v>107</v>
+      </c>
+      <c r="I8">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="J8">
+        <v>256</v>
+      </c>
+      <c r="K8">
+        <v>197</v>
+      </c>
+      <c r="L8">
+        <v>2</v>
+      </c>
+      <c r="M8">
+        <v>2</v>
+      </c>
+      <c r="N8">
+        <v>0.77</v>
+      </c>
+      <c r="O8">
+        <v>0.05</v>
+      </c>
+      <c r="P8">
+        <v>5.52</v>
+      </c>
+      <c r="Q8">
+        <v>157</v>
+      </c>
+      <c r="R8">
+        <v>138</v>
+      </c>
+      <c r="S8">
+        <v>92</v>
+      </c>
+      <c r="T8">
+        <v>410</v>
+      </c>
+      <c r="U8">
+        <v>22.44</v>
+      </c>
+      <c r="V8">
+        <v>55</v>
+      </c>
+      <c r="W8">
+        <v>330</v>
+      </c>
+      <c r="X8">
+        <v>83.33</v>
+      </c>
+      <c r="Y8">
+        <v>7</v>
+      </c>
+      <c r="Z8">
+        <v>4</v>
+      </c>
+      <c r="AA8">
+        <v>11.6</v>
+      </c>
+      <c r="AB8">
+        <v>14.2</v>
+      </c>
+      <c r="AC8">
+        <v>2346</v>
+      </c>
+      <c r="AD8">
+        <v>10.9</v>
+      </c>
+      <c r="AE8">
+        <v>2148</v>
+      </c>
+      <c r="AF8">
+        <v>0.90800000000000003</v>
+      </c>
+      <c r="AG8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9">
+        <v>30</v>
+      </c>
+      <c r="D9">
+        <v>82</v>
+      </c>
+      <c r="E9">
+        <v>50</v>
+      </c>
+      <c r="F9">
+        <v>25</v>
+      </c>
+      <c r="G9">
+        <v>7</v>
+      </c>
+      <c r="H9">
+        <v>107</v>
+      </c>
+      <c r="I9">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="J9">
+        <v>217</v>
+      </c>
+      <c r="K9">
+        <v>195</v>
+      </c>
+      <c r="L9">
+        <v>9</v>
+      </c>
+      <c r="M9">
+        <v>4</v>
+      </c>
+      <c r="N9">
+        <v>0.44</v>
+      </c>
+      <c r="O9">
+        <v>0.08</v>
+      </c>
+      <c r="P9">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="Q9">
+        <v>135</v>
+      </c>
+      <c r="R9">
+        <v>129</v>
+      </c>
+      <c r="S9">
+        <v>79</v>
+      </c>
+      <c r="T9">
+        <v>427</v>
+      </c>
+      <c r="U9">
+        <v>18.5</v>
+      </c>
+      <c r="V9">
+        <v>59</v>
+      </c>
+      <c r="W9">
+        <v>377</v>
+      </c>
+      <c r="X9">
+        <v>84.35</v>
+      </c>
+      <c r="Y9">
+        <v>3</v>
+      </c>
+      <c r="Z9">
+        <v>6</v>
+      </c>
+      <c r="AA9">
+        <v>13.8</v>
+      </c>
+      <c r="AB9">
+        <v>14.9</v>
+      </c>
+      <c r="AC9">
+        <v>2295</v>
+      </c>
+      <c r="AD9">
+        <v>9.5</v>
+      </c>
+      <c r="AE9">
+        <v>2114</v>
+      </c>
+      <c r="AF9">
+        <v>0.90800000000000003</v>
+      </c>
+      <c r="AG9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10">
+        <v>26</v>
+      </c>
+      <c r="D10">
+        <v>82</v>
+      </c>
+      <c r="E10">
+        <v>47</v>
+      </c>
+      <c r="F10">
+        <v>24</v>
+      </c>
+      <c r="G10">
+        <v>11</v>
+      </c>
+      <c r="H10">
+        <v>105</v>
+      </c>
+      <c r="I10">
+        <v>0.64</v>
+      </c>
+      <c r="J10">
+        <v>267</v>
+      </c>
+      <c r="K10">
+        <v>240</v>
+      </c>
+      <c r="L10">
+        <v>10</v>
+      </c>
+      <c r="M10">
+        <v>6</v>
+      </c>
+      <c r="N10">
+        <v>0.21</v>
+      </c>
+      <c r="O10">
+        <v>-0.17</v>
+      </c>
+      <c r="P10">
+        <v>6.18</v>
+      </c>
+      <c r="Q10">
+        <v>159</v>
+      </c>
+      <c r="R10">
+        <v>152</v>
+      </c>
+      <c r="S10">
+        <v>94</v>
+      </c>
+      <c r="T10">
+        <v>463</v>
+      </c>
+      <c r="U10">
+        <v>20.3</v>
+      </c>
+      <c r="V10">
+        <v>75</v>
+      </c>
+      <c r="W10">
+        <v>419</v>
+      </c>
+      <c r="X10">
+        <v>82.1</v>
+      </c>
+      <c r="Y10">
+        <v>14</v>
+      </c>
+      <c r="Z10">
+        <v>13</v>
+      </c>
+      <c r="AA10">
+        <v>15.2</v>
+      </c>
+      <c r="AB10">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="AC10">
+        <v>2366</v>
+      </c>
+      <c r="AD10">
+        <v>11.3</v>
+      </c>
+      <c r="AE10">
+        <v>2529</v>
+      </c>
+      <c r="AF10">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="AG10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11">
+        <v>26.6</v>
+      </c>
+      <c r="D11">
+        <v>82</v>
+      </c>
+      <c r="E11">
+        <v>48</v>
+      </c>
+      <c r="F11">
+        <v>25</v>
+      </c>
+      <c r="G11">
+        <v>9</v>
+      </c>
+      <c r="H11">
+        <v>105</v>
+      </c>
+      <c r="I11">
+        <v>0.64</v>
+      </c>
+      <c r="J11">
+        <v>286</v>
+      </c>
+      <c r="K11">
+        <v>216</v>
+      </c>
+      <c r="L11">
+        <v>2</v>
+      </c>
+      <c r="M11">
+        <v>6</v>
+      </c>
+      <c r="N11">
+        <v>0.64</v>
+      </c>
+      <c r="O11">
+        <v>-0.16</v>
+      </c>
+      <c r="P11">
+        <v>6.12</v>
+      </c>
+      <c r="Q11">
+        <v>197</v>
+      </c>
+      <c r="R11">
+        <v>143</v>
+      </c>
+      <c r="S11">
+        <v>72</v>
+      </c>
+      <c r="T11">
+        <v>403</v>
+      </c>
+      <c r="U11">
+        <v>17.87</v>
+      </c>
+      <c r="V11">
+        <v>61</v>
+      </c>
+      <c r="W11">
+        <v>394</v>
+      </c>
+      <c r="X11">
+        <v>84.52</v>
+      </c>
+      <c r="Y11">
+        <v>17</v>
+      </c>
+      <c r="Z11">
+        <v>12</v>
+      </c>
+      <c r="AA11">
+        <v>14.2</v>
+      </c>
+      <c r="AB11">
+        <v>14.6</v>
+      </c>
+      <c r="AC11">
+        <v>2651</v>
+      </c>
+      <c r="AD11">
+        <v>10.8</v>
+      </c>
+      <c r="AE11">
+        <v>2479</v>
+      </c>
+      <c r="AF11">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="AG11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12">
+        <v>28</v>
+      </c>
+      <c r="D12">
+        <v>82</v>
+      </c>
+      <c r="E12">
+        <v>49</v>
+      </c>
+      <c r="F12">
+        <v>26</v>
+      </c>
+      <c r="G12">
+        <v>7</v>
+      </c>
+      <c r="H12">
+        <v>105</v>
+      </c>
+      <c r="I12">
+        <v>0.64</v>
+      </c>
+      <c r="J12">
+        <v>217</v>
+      </c>
+      <c r="K12">
+        <v>197</v>
+      </c>
+      <c r="L12">
+        <v>5</v>
+      </c>
+      <c r="M12">
+        <v>4</v>
+      </c>
+      <c r="N12">
+        <v>0.39</v>
+      </c>
+      <c r="O12">
+        <v>0.13</v>
+      </c>
+      <c r="P12">
+        <v>5.05</v>
+      </c>
+      <c r="Q12">
+        <v>142</v>
+      </c>
+      <c r="R12">
+        <v>132</v>
+      </c>
+      <c r="S12">
+        <v>70</v>
+      </c>
+      <c r="T12">
+        <v>407</v>
+      </c>
+      <c r="U12">
+        <v>17.2</v>
+      </c>
+      <c r="V12">
+        <v>57</v>
+      </c>
+      <c r="W12">
+        <v>436</v>
+      </c>
+      <c r="X12">
+        <v>86.93</v>
+      </c>
+      <c r="Y12">
+        <v>5</v>
+      </c>
+      <c r="Z12">
+        <v>8</v>
+      </c>
+      <c r="AA12">
+        <v>14.7</v>
+      </c>
+      <c r="AB12">
+        <v>14.2</v>
+      </c>
+      <c r="AC12">
+        <v>2405</v>
+      </c>
+      <c r="AD12">
+        <v>9</v>
+      </c>
+      <c r="AE12">
+        <v>2398</v>
+      </c>
+      <c r="AF12">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="AG12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33">
+      <c r="A13" s="2">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13">
+        <v>28.2</v>
+      </c>
+      <c r="D13">
+        <v>82</v>
+      </c>
+      <c r="E13">
+        <v>48</v>
+      </c>
+      <c r="F13">
+        <v>26</v>
+      </c>
+      <c r="G13">
+        <v>8</v>
+      </c>
+      <c r="H13">
+        <v>104</v>
+      </c>
+      <c r="I13">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="J13">
+        <v>225</v>
+      </c>
+      <c r="K13">
+        <v>184</v>
+      </c>
+      <c r="L13">
+        <v>10</v>
+      </c>
+      <c r="M13">
+        <v>7</v>
+      </c>
+      <c r="N13">
+        <v>0.65</v>
+      </c>
+      <c r="O13">
+        <v>0.11</v>
+      </c>
+      <c r="P13">
+        <v>4.99</v>
+      </c>
+      <c r="Q13">
+        <v>144</v>
+      </c>
+      <c r="R13">
+        <v>128</v>
+      </c>
+      <c r="S13">
+        <v>72</v>
+      </c>
+      <c r="T13">
+        <v>380</v>
+      </c>
+      <c r="U13">
+        <v>18.95</v>
+      </c>
+      <c r="V13">
+        <v>48</v>
+      </c>
+      <c r="W13">
+        <v>342</v>
+      </c>
+      <c r="X13">
+        <v>85.96</v>
+      </c>
+      <c r="Y13">
+        <v>9</v>
+      </c>
+      <c r="Z13">
+        <v>8</v>
+      </c>
+      <c r="AA13">
+        <v>10.5</v>
+      </c>
+      <c r="AB13">
+        <v>11.6</v>
+      </c>
+      <c r="AC13">
+        <v>2431</v>
+      </c>
+      <c r="AD13">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="AE13">
+        <v>2361</v>
+      </c>
+      <c r="AF13">
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="AG13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33">
+      <c r="A14" s="2">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C14">
+        <v>29.4</v>
+      </c>
+      <c r="D14">
+        <v>82</v>
+      </c>
+      <c r="E14">
+        <v>43</v>
+      </c>
+      <c r="F14">
+        <v>28</v>
+      </c>
+      <c r="G14">
+        <v>11</v>
+      </c>
+      <c r="H14">
+        <v>97</v>
+      </c>
+      <c r="I14">
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="J14">
+        <v>239</v>
+      </c>
+      <c r="K14">
+        <v>241</v>
+      </c>
+      <c r="L14">
+        <v>7</v>
+      </c>
+      <c r="M14">
+        <v>4</v>
+      </c>
+      <c r="N14">
+        <v>-0.15</v>
+      </c>
+      <c r="O14">
+        <v>-0.16</v>
+      </c>
+      <c r="P14">
+        <v>5.85</v>
+      </c>
+      <c r="Q14">
+        <v>163</v>
+      </c>
+      <c r="R14">
+        <v>152</v>
+      </c>
+      <c r="S14">
+        <v>67</v>
+      </c>
+      <c r="T14">
+        <v>407</v>
+      </c>
+      <c r="U14">
+        <v>16.46</v>
+      </c>
+      <c r="V14">
+        <v>79</v>
+      </c>
+      <c r="W14">
+        <v>391</v>
+      </c>
+      <c r="X14">
+        <v>79.8</v>
+      </c>
+      <c r="Y14">
+        <v>9</v>
+      </c>
+      <c r="Z14">
+        <v>10</v>
+      </c>
+      <c r="AA14">
+        <v>13.4</v>
+      </c>
+      <c r="AB14">
+        <v>14</v>
+      </c>
+      <c r="AC14">
+        <v>2438</v>
+      </c>
+      <c r="AD14">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="AE14">
+        <v>2582</v>
+      </c>
+      <c r="AF14">
+        <v>0.90700000000000003</v>
+      </c>
+      <c r="AG14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33">
+      <c r="A15" s="2">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15">
+        <v>28.4</v>
+      </c>
+      <c r="D15">
+        <v>82</v>
+      </c>
+      <c r="E15">
+        <v>43</v>
+      </c>
+      <c r="F15">
+        <v>29</v>
+      </c>
+      <c r="G15">
+        <v>10</v>
+      </c>
+      <c r="H15">
+        <v>96</v>
+      </c>
+      <c r="I15">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="J15">
+        <v>255</v>
+      </c>
+      <c r="K15">
+        <v>221</v>
+      </c>
+      <c r="L15">
+        <v>3</v>
+      </c>
+      <c r="M15">
+        <v>5</v>
+      </c>
+      <c r="N15">
+        <v>0.51</v>
+      </c>
+      <c r="O15">
+        <v>0.12</v>
+      </c>
+      <c r="P15">
+        <v>5.8</v>
+      </c>
+      <c r="Q15">
+        <v>167</v>
+      </c>
+      <c r="R15">
+        <v>135</v>
+      </c>
+      <c r="S15">
+        <v>73</v>
+      </c>
+      <c r="T15">
+        <v>401</v>
+      </c>
+      <c r="U15">
+        <v>18.2</v>
+      </c>
+      <c r="V15">
+        <v>81</v>
+      </c>
+      <c r="W15">
+        <v>414</v>
+      </c>
+      <c r="X15">
+        <v>80.430000000000007</v>
+      </c>
+      <c r="Y15">
+        <v>15</v>
+      </c>
+      <c r="Z15">
+        <v>5</v>
+      </c>
+      <c r="AA15">
+        <v>14.7</v>
+      </c>
+      <c r="AB15">
+        <v>14.3</v>
+      </c>
+      <c r="AC15">
+        <v>2242</v>
+      </c>
+      <c r="AD15">
+        <v>11.4</v>
+      </c>
+      <c r="AE15">
+        <v>2502</v>
+      </c>
+      <c r="AF15">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="AG15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33">
+      <c r="A16" s="2">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16">
+        <v>28.4</v>
+      </c>
+      <c r="D16">
+        <v>82</v>
+      </c>
+      <c r="E16">
+        <v>44</v>
+      </c>
+      <c r="F16">
+        <v>31</v>
+      </c>
+      <c r="G16">
+        <v>7</v>
+      </c>
+      <c r="H16">
+        <v>95</v>
+      </c>
+      <c r="I16">
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="J16">
+        <v>267</v>
+      </c>
+      <c r="K16">
+        <v>247</v>
+      </c>
+      <c r="L16">
+        <v>5</v>
+      </c>
+      <c r="M16">
+        <v>4</v>
+      </c>
+      <c r="N16">
+        <v>0.39</v>
+      </c>
+      <c r="O16">
+        <v>0.13</v>
+      </c>
+      <c r="P16">
+        <v>6.27</v>
+      </c>
+      <c r="Q16">
+        <v>181</v>
+      </c>
+      <c r="R16">
+        <v>168</v>
+      </c>
+      <c r="S16">
+        <v>79</v>
+      </c>
+      <c r="T16">
+        <v>374</v>
+      </c>
+      <c r="U16">
+        <v>21.12</v>
+      </c>
+      <c r="V16">
+        <v>70</v>
+      </c>
+      <c r="W16">
+        <v>353</v>
+      </c>
+      <c r="X16">
+        <v>80.17</v>
+      </c>
+      <c r="Y16">
+        <v>7</v>
+      </c>
+      <c r="Z16">
+        <v>9</v>
+      </c>
+      <c r="AA16">
+        <v>10.8</v>
+      </c>
+      <c r="AB16">
+        <v>11.6</v>
+      </c>
+      <c r="AC16">
+        <v>2603</v>
+      </c>
+      <c r="AD16">
+        <v>10.3</v>
+      </c>
+      <c r="AE16">
+        <v>2378</v>
+      </c>
+      <c r="AF16">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="AG16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33">
+      <c r="A17" s="2">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17">
+        <v>28.6</v>
+      </c>
+      <c r="D17">
+        <v>82</v>
+      </c>
+      <c r="E17">
+        <v>42</v>
+      </c>
+      <c r="F17">
+        <v>30</v>
+      </c>
+      <c r="G17">
+        <v>10</v>
+      </c>
+      <c r="H17">
+        <v>94</v>
+      </c>
+      <c r="I17">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="J17">
+        <v>233</v>
+      </c>
+      <c r="K17">
+        <v>211</v>
+      </c>
+      <c r="L17">
+        <v>9</v>
+      </c>
+      <c r="M17">
+        <v>5</v>
+      </c>
+      <c r="N17">
+        <v>0.16</v>
+      </c>
+      <c r="O17">
+        <v>-0.16</v>
+      </c>
+      <c r="P17">
+        <v>5.41</v>
+      </c>
+      <c r="Q17">
+        <v>147</v>
+      </c>
+      <c r="R17">
+        <v>140</v>
+      </c>
+      <c r="S17">
+        <v>75</v>
+      </c>
+      <c r="T17">
+        <v>406</v>
+      </c>
+      <c r="U17">
+        <v>18.47</v>
+      </c>
+      <c r="V17">
+        <v>65</v>
+      </c>
+      <c r="W17">
+        <v>400</v>
+      </c>
+      <c r="X17">
+        <v>83.75</v>
+      </c>
+      <c r="Y17">
+        <v>11</v>
+      </c>
+      <c r="Z17">
+        <v>6</v>
+      </c>
+      <c r="AA17">
+        <v>13.5</v>
+      </c>
+      <c r="AB17">
+        <v>14.3</v>
+      </c>
+      <c r="AC17">
+        <v>2586</v>
+      </c>
+      <c r="AD17">
+        <v>9</v>
+      </c>
+      <c r="AE17">
+        <v>2329</v>
+      </c>
+      <c r="AF17">
+        <v>0.90900000000000003</v>
+      </c>
+      <c r="AG17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33">
+      <c r="A18" s="2">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18">
+        <v>28.2</v>
+      </c>
+      <c r="D18">
+        <v>82</v>
+      </c>
+      <c r="E18">
+        <v>44</v>
+      </c>
+      <c r="F18">
+        <v>33</v>
+      </c>
+      <c r="G18">
+        <v>5</v>
+      </c>
+      <c r="H18">
+        <v>93</v>
+      </c>
+      <c r="I18">
+        <v>0.56699999999999995</v>
+      </c>
+      <c r="J18">
+        <v>243</v>
+      </c>
+      <c r="K18">
+        <v>259</v>
+      </c>
+      <c r="L18">
+        <v>10</v>
+      </c>
+      <c r="M18">
+        <v>2</v>
+      </c>
+      <c r="N18">
+        <v>-0.25</v>
+      </c>
+      <c r="O18">
+        <v>-0.15</v>
+      </c>
+      <c r="P18">
+        <v>6.12</v>
+      </c>
+      <c r="Q18">
+        <v>160</v>
+      </c>
+      <c r="R18">
+        <v>182</v>
+      </c>
+      <c r="S18">
+        <v>69</v>
+      </c>
+      <c r="T18">
+        <v>374</v>
+      </c>
+      <c r="U18">
+        <v>18.45</v>
+      </c>
+      <c r="V18">
+        <v>66</v>
+      </c>
+      <c r="W18">
+        <v>305</v>
+      </c>
+      <c r="X18">
+        <v>78.36</v>
+      </c>
+      <c r="Y18">
+        <v>14</v>
+      </c>
+      <c r="Z18">
+        <v>11</v>
+      </c>
+      <c r="AA18">
+        <v>10.9</v>
+      </c>
+      <c r="AB18">
+        <v>12.9</v>
+      </c>
+      <c r="AC18">
+        <v>2418</v>
+      </c>
+      <c r="AD18">
+        <v>10</v>
+      </c>
+      <c r="AE18">
+        <v>2234</v>
+      </c>
+      <c r="AF18">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="AG18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33">
+      <c r="A19" s="2">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19">
+        <v>29.7</v>
+      </c>
+      <c r="D19">
+        <v>82</v>
+      </c>
+      <c r="E19">
+        <v>40</v>
+      </c>
+      <c r="F19">
+        <v>30</v>
+      </c>
+      <c r="G19">
+        <v>12</v>
+      </c>
+      <c r="H19">
+        <v>92</v>
+      </c>
+      <c r="I19">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="J19">
+        <v>240</v>
+      </c>
+      <c r="K19">
+        <v>235</v>
+      </c>
+      <c r="L19">
+        <v>8</v>
+      </c>
+      <c r="M19">
+        <v>5</v>
+      </c>
+      <c r="N19">
+        <v>-0.04</v>
+      </c>
+      <c r="O19">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="P19">
+        <v>5.79</v>
+      </c>
+      <c r="Q19">
+        <v>170</v>
+      </c>
+      <c r="R19">
+        <v>147</v>
+      </c>
+      <c r="S19">
+        <v>63</v>
+      </c>
+      <c r="T19">
+        <v>348</v>
+      </c>
+      <c r="U19">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="V19">
+        <v>79</v>
+      </c>
+      <c r="W19">
+        <v>433</v>
+      </c>
+      <c r="X19">
+        <v>81.760000000000005</v>
+      </c>
+      <c r="Y19">
+        <v>7</v>
+      </c>
+      <c r="Z19">
+        <v>9</v>
+      </c>
+      <c r="AA19">
+        <v>12.9</v>
+      </c>
+      <c r="AB19">
+        <v>11.1</v>
+      </c>
+      <c r="AC19">
+        <v>2457</v>
+      </c>
+      <c r="AD19">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="AE19">
+        <v>2671</v>
+      </c>
+      <c r="AF19">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="AG19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33">
+      <c r="A20" s="2">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20">
+        <v>27.8</v>
+      </c>
+      <c r="D20">
+        <v>82</v>
+      </c>
+      <c r="E20">
+        <v>40</v>
+      </c>
+      <c r="F20">
+        <v>31</v>
+      </c>
+      <c r="G20">
+        <v>11</v>
+      </c>
+      <c r="H20">
+        <v>91</v>
+      </c>
+      <c r="I20">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="J20">
+        <v>254</v>
+      </c>
+      <c r="K20">
+        <v>262</v>
+      </c>
+      <c r="L20">
+        <v>4</v>
+      </c>
+      <c r="M20">
+        <v>7</v>
+      </c>
+      <c r="N20">
+        <v>-0.21</v>
+      </c>
+      <c r="O20">
+        <v>-0.08</v>
+      </c>
+      <c r="P20">
+        <v>6.29</v>
+      </c>
+      <c r="Q20">
+        <v>180</v>
+      </c>
+      <c r="R20">
+        <v>161</v>
+      </c>
+      <c r="S20">
+        <v>71</v>
+      </c>
+      <c r="T20">
+        <v>401</v>
+      </c>
+      <c r="U20">
+        <v>17.71</v>
+      </c>
+      <c r="V20">
+        <v>90</v>
+      </c>
+      <c r="W20">
+        <v>418</v>
+      </c>
+      <c r="X20">
+        <v>78.47</v>
+      </c>
+      <c r="Y20">
+        <v>3</v>
+      </c>
+      <c r="Z20">
+        <v>11</v>
+      </c>
+      <c r="AA20">
+        <v>13.9</v>
+      </c>
+      <c r="AB20">
+        <v>13.2</v>
+      </c>
+      <c r="AC20">
+        <v>2681</v>
+      </c>
+      <c r="AD20">
+        <v>9.5</v>
+      </c>
+      <c r="AE20">
+        <v>2330</v>
+      </c>
+      <c r="AF20">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="AG20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33">
+      <c r="A21" s="2">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21">
+        <v>28</v>
+      </c>
+      <c r="D21">
+        <v>82</v>
+      </c>
+      <c r="E21">
+        <v>42</v>
+      </c>
+      <c r="F21">
+        <v>34</v>
+      </c>
+      <c r="G21">
+        <v>6</v>
+      </c>
+      <c r="H21">
+        <v>90</v>
+      </c>
+      <c r="I21">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="J21">
+        <v>239</v>
+      </c>
+      <c r="K21">
+        <v>251</v>
+      </c>
+      <c r="L21">
+        <v>6</v>
+      </c>
+      <c r="M21">
+        <v>5</v>
+      </c>
+      <c r="N21">
+        <v>-0.21</v>
+      </c>
+      <c r="O21">
+        <v>-0.08</v>
+      </c>
+      <c r="P21">
+        <v>5.98</v>
+      </c>
+      <c r="Q21">
+        <v>136</v>
+      </c>
+      <c r="R21">
+        <v>176</v>
+      </c>
+      <c r="S21">
+        <v>86</v>
+      </c>
+      <c r="T21">
+        <v>378</v>
+      </c>
+      <c r="U21">
+        <v>22.75</v>
+      </c>
+      <c r="V21">
+        <v>69</v>
+      </c>
+      <c r="W21">
+        <v>419</v>
+      </c>
+      <c r="X21">
+        <v>83.53</v>
+      </c>
+      <c r="Y21">
+        <v>17</v>
+      </c>
+      <c r="Z21">
+        <v>6</v>
+      </c>
+      <c r="AA21">
+        <v>13.8</v>
+      </c>
+      <c r="AB21">
+        <v>13.1</v>
+      </c>
+      <c r="AC21">
+        <v>2426</v>
+      </c>
+      <c r="AD21">
+        <v>9.9</v>
+      </c>
+      <c r="AE21">
+        <v>2685</v>
+      </c>
+      <c r="AF21">
+        <v>0.90700000000000003</v>
+      </c>
+      <c r="AG21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33">
+      <c r="A22" s="2">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22">
+        <v>28.2</v>
+      </c>
+      <c r="D22">
+        <v>82</v>
+      </c>
+      <c r="E22">
+        <v>40</v>
+      </c>
+      <c r="F22">
+        <v>34</v>
+      </c>
+      <c r="G22">
+        <v>8</v>
+      </c>
+      <c r="H22">
+        <v>88</v>
+      </c>
+      <c r="I22">
+        <v>0.53700000000000003</v>
+      </c>
+      <c r="J22">
+        <v>241</v>
+      </c>
+      <c r="K22">
+        <v>248</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>5</v>
+      </c>
+      <c r="N22">
+        <v>-0.28999999999999998</v>
+      </c>
+      <c r="O22">
+        <v>-0.15</v>
+      </c>
+      <c r="P22">
+        <v>5.96</v>
+      </c>
+      <c r="Q22">
+        <v>162</v>
+      </c>
+      <c r="R22">
+        <v>179</v>
+      </c>
+      <c r="S22">
+        <v>67</v>
+      </c>
+      <c r="T22">
+        <v>447</v>
+      </c>
+      <c r="U22">
+        <v>14.99</v>
+      </c>
+      <c r="V22">
+        <v>61</v>
+      </c>
+      <c r="W22">
+        <v>395</v>
+      </c>
+      <c r="X22">
+        <v>84.56</v>
+      </c>
+      <c r="Y22">
+        <v>12</v>
+      </c>
+      <c r="Z22">
+        <v>8</v>
+      </c>
+      <c r="AA22">
+        <v>12.5</v>
+      </c>
+      <c r="AB22">
+        <v>14.1</v>
+      </c>
+      <c r="AC22">
+        <v>2559</v>
+      </c>
+      <c r="AD22">
+        <v>9.4</v>
+      </c>
+      <c r="AE22">
+        <v>2336</v>
+      </c>
+      <c r="AF22">
+        <v>0.89400000000000002</v>
+      </c>
+      <c r="AG22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33">
+      <c r="A23" s="2">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23">
+        <v>29.1</v>
+      </c>
+      <c r="D23">
+        <v>82</v>
+      </c>
+      <c r="E23">
+        <v>35</v>
+      </c>
+      <c r="F23">
+        <v>31</v>
+      </c>
+      <c r="G23">
+        <v>16</v>
+      </c>
+      <c r="H23">
+        <v>86</v>
+      </c>
+      <c r="I23">
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="J23">
+        <v>245</v>
+      </c>
+      <c r="K23">
+        <v>249</v>
+      </c>
+      <c r="L23">
+        <v>2</v>
+      </c>
+      <c r="M23">
+        <v>8</v>
+      </c>
+      <c r="N23">
+        <v>-0.27</v>
+      </c>
+      <c r="O23">
+        <v>-0.15</v>
+      </c>
+      <c r="P23">
+        <v>6.02</v>
+      </c>
+      <c r="Q23">
+        <v>179</v>
+      </c>
+      <c r="R23">
+        <v>165</v>
+      </c>
+      <c r="S23">
+        <v>61</v>
+      </c>
+      <c r="T23">
+        <v>337</v>
+      </c>
+      <c r="U23">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="V23">
+        <v>78</v>
+      </c>
+      <c r="W23">
+        <v>443</v>
+      </c>
+      <c r="X23">
+        <v>82.39</v>
+      </c>
+      <c r="Y23">
+        <v>5</v>
+      </c>
+      <c r="Z23">
+        <v>6</v>
+      </c>
+      <c r="AA23">
+        <v>14.4</v>
+      </c>
+      <c r="AB23">
+        <v>11.4</v>
+      </c>
+      <c r="AC23">
+        <v>2730</v>
+      </c>
+      <c r="AD23">
+        <v>9</v>
+      </c>
+      <c r="AE23">
+        <v>2402</v>
+      </c>
+      <c r="AF23">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="AG23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33">
+      <c r="A24" s="2">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24">
+        <v>28.9</v>
+      </c>
+      <c r="D24">
+        <v>82</v>
+      </c>
+      <c r="E24">
+        <v>34</v>
+      </c>
+      <c r="F24">
+        <v>35</v>
+      </c>
+      <c r="G24">
+        <v>13</v>
+      </c>
+      <c r="H24">
+        <v>81</v>
+      </c>
+      <c r="I24">
+        <v>0.49399999999999999</v>
+      </c>
+      <c r="J24">
+        <v>208</v>
+      </c>
+      <c r="K24">
+        <v>248</v>
+      </c>
+      <c r="L24">
+        <v>6</v>
+      </c>
+      <c r="M24">
+        <v>6</v>
+      </c>
+      <c r="N24">
+        <v>-0.33</v>
+      </c>
+      <c r="O24">
+        <v>0.15</v>
+      </c>
+      <c r="P24">
+        <v>5.56</v>
+      </c>
+      <c r="Q24">
+        <v>155</v>
+      </c>
+      <c r="R24">
+        <v>155</v>
+      </c>
+      <c r="S24">
+        <v>46</v>
+      </c>
+      <c r="T24">
+        <v>381</v>
+      </c>
+      <c r="U24">
+        <v>12.07</v>
+      </c>
+      <c r="V24">
+        <v>83</v>
+      </c>
+      <c r="W24">
+        <v>414</v>
+      </c>
+      <c r="X24">
+        <v>79.95</v>
+      </c>
+      <c r="Y24">
+        <v>7</v>
+      </c>
+      <c r="Z24">
+        <v>10</v>
+      </c>
+      <c r="AA24">
+        <v>14.9</v>
+      </c>
+      <c r="AB24">
+        <v>13.4</v>
+      </c>
+      <c r="AC24">
+        <v>2202</v>
+      </c>
+      <c r="AD24">
+        <v>9.4</v>
+      </c>
+      <c r="AE24">
+        <v>2369</v>
+      </c>
+      <c r="AF24">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="AG24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33">
+      <c r="A25" s="2">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25">
+        <v>27.8</v>
+      </c>
+      <c r="D25">
+        <v>82</v>
+      </c>
+      <c r="E25">
+        <v>35</v>
+      </c>
+      <c r="F25">
+        <v>41</v>
+      </c>
+      <c r="G25">
+        <v>6</v>
+      </c>
+      <c r="H25">
+        <v>76</v>
+      </c>
+      <c r="I25">
+        <v>0.46300000000000002</v>
+      </c>
+      <c r="J25">
+        <v>210</v>
+      </c>
+      <c r="K25">
+        <v>285</v>
+      </c>
+      <c r="L25">
+        <v>9</v>
+      </c>
+      <c r="M25">
+        <v>4</v>
+      </c>
+      <c r="N25">
+        <v>-0.87</v>
+      </c>
+      <c r="O25">
+        <v>-0.01</v>
+      </c>
+      <c r="P25">
+        <v>6.04</v>
+      </c>
+      <c r="Q25">
+        <v>131</v>
+      </c>
+      <c r="R25">
+        <v>186</v>
+      </c>
+      <c r="S25">
+        <v>71</v>
+      </c>
+      <c r="T25">
+        <v>412</v>
+      </c>
+      <c r="U25">
+        <v>17.23</v>
+      </c>
+      <c r="V25">
+        <v>81</v>
+      </c>
+      <c r="W25">
+        <v>442</v>
+      </c>
+      <c r="X25">
+        <v>81.67</v>
+      </c>
+      <c r="Y25">
+        <v>8</v>
+      </c>
+      <c r="Z25">
+        <v>18</v>
+      </c>
+      <c r="AA25">
+        <v>15.3</v>
+      </c>
+      <c r="AB25">
+        <v>14.5</v>
+      </c>
+      <c r="AC25">
+        <v>2370</v>
+      </c>
+      <c r="AD25">
+        <v>8.9</v>
+      </c>
+      <c r="AE25">
+        <v>2748</v>
+      </c>
+      <c r="AF25">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="AG25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33">
+      <c r="A26" s="2">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26">
+        <v>27.8</v>
+      </c>
+      <c r="D26">
+        <v>82</v>
+      </c>
+      <c r="E26">
+        <v>33</v>
+      </c>
+      <c r="F26">
+        <v>42</v>
+      </c>
+      <c r="G26">
+        <v>7</v>
+      </c>
+      <c r="H26">
+        <v>73</v>
+      </c>
+      <c r="I26">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="J26">
+        <v>196</v>
+      </c>
+      <c r="K26">
+        <v>244</v>
+      </c>
+      <c r="L26">
+        <v>5</v>
+      </c>
+      <c r="M26">
+        <v>5</v>
+      </c>
+      <c r="N26">
+        <v>-0.42</v>
+      </c>
+      <c r="O26">
+        <v>0.16</v>
+      </c>
+      <c r="P26">
+        <v>5.37</v>
+      </c>
+      <c r="Q26">
+        <v>125</v>
+      </c>
+      <c r="R26">
+        <v>149</v>
+      </c>
+      <c r="S26">
+        <v>65</v>
+      </c>
+      <c r="T26">
+        <v>438</v>
+      </c>
+      <c r="U26">
+        <v>14.84</v>
+      </c>
+      <c r="V26">
+        <v>85</v>
+      </c>
+      <c r="W26">
+        <v>453</v>
+      </c>
+      <c r="X26">
+        <v>81.239999999999995</v>
+      </c>
+      <c r="Y26">
+        <v>6</v>
+      </c>
+      <c r="Z26">
+        <v>10</v>
+      </c>
+      <c r="AA26">
+        <v>16.5</v>
+      </c>
+      <c r="AB26">
+        <v>16</v>
+      </c>
+      <c r="AC26">
+        <v>2273</v>
+      </c>
+      <c r="AD26">
+        <v>8.6</v>
+      </c>
+      <c r="AE26">
+        <v>2345</v>
+      </c>
+      <c r="AF26">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="AG26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:33">
+      <c r="A27" s="2">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27">
+        <v>28.2</v>
+      </c>
+      <c r="D27">
+        <v>82</v>
+      </c>
+      <c r="E27">
+        <v>32</v>
+      </c>
+      <c r="F27">
+        <v>43</v>
+      </c>
+      <c r="G27">
+        <v>7</v>
+      </c>
+      <c r="H27">
+        <v>71</v>
+      </c>
+      <c r="I27">
+        <v>0.433</v>
+      </c>
+      <c r="J27">
+        <v>192</v>
+      </c>
+      <c r="K27">
+        <v>245</v>
+      </c>
+      <c r="L27">
+        <v>3</v>
+      </c>
+      <c r="M27">
+        <v>3</v>
+      </c>
+      <c r="N27">
+        <v>-0.43</v>
+      </c>
+      <c r="O27">
+        <v>0.22</v>
+      </c>
+      <c r="P27">
+        <v>5.33</v>
+      </c>
+      <c r="Q27">
+        <v>133</v>
+      </c>
+      <c r="R27">
+        <v>182</v>
+      </c>
+      <c r="S27">
+        <v>53</v>
+      </c>
+      <c r="T27">
+        <v>373</v>
+      </c>
+      <c r="U27">
+        <v>14.21</v>
+      </c>
+      <c r="V27">
+        <v>59</v>
+      </c>
+      <c r="W27">
+        <v>382</v>
+      </c>
+      <c r="X27">
+        <v>84.55</v>
+      </c>
+      <c r="Y27">
+        <v>6</v>
+      </c>
+      <c r="Z27">
+        <v>4</v>
+      </c>
+      <c r="AA27">
+        <v>15.7</v>
+      </c>
+      <c r="AB27">
+        <v>14.6</v>
+      </c>
+      <c r="AC27">
+        <v>2193</v>
+      </c>
+      <c r="AD27">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="AE27">
+        <v>2439</v>
+      </c>
+      <c r="AF27">
+        <v>0.9</v>
+      </c>
+      <c r="AG27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33">
+      <c r="A28" s="2">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28">
+        <v>27.5</v>
+      </c>
+      <c r="D28">
+        <v>82</v>
+      </c>
+      <c r="E28">
+        <v>31</v>
+      </c>
+      <c r="F28">
+        <v>42</v>
+      </c>
+      <c r="G28">
+        <v>9</v>
+      </c>
+      <c r="H28">
+        <v>71</v>
+      </c>
+      <c r="I28">
+        <v>0.433</v>
+      </c>
+      <c r="J28">
+        <v>195</v>
+      </c>
+      <c r="K28">
+        <v>251</v>
+      </c>
+      <c r="L28">
+        <v>6</v>
+      </c>
+      <c r="M28">
+        <v>7</v>
+      </c>
+      <c r="N28">
+        <v>-0.52</v>
+      </c>
+      <c r="O28">
+        <v>0.17</v>
+      </c>
+      <c r="P28">
+        <v>5.44</v>
+      </c>
+      <c r="Q28">
+        <v>140</v>
+      </c>
+      <c r="R28">
+        <v>168</v>
+      </c>
+      <c r="S28">
+        <v>43</v>
+      </c>
+      <c r="T28">
+        <v>364</v>
+      </c>
+      <c r="U28">
+        <v>11.81</v>
+      </c>
+      <c r="V28">
+        <v>77</v>
+      </c>
+      <c r="W28">
+        <v>443</v>
+      </c>
+      <c r="X28">
+        <v>82.62</v>
+      </c>
+      <c r="Y28">
+        <v>12</v>
+      </c>
+      <c r="Z28">
+        <v>6</v>
+      </c>
+      <c r="AA28">
+        <v>16.2</v>
+      </c>
+      <c r="AB28">
+        <v>13.7</v>
+      </c>
+      <c r="AC28">
+        <v>2201</v>
+      </c>
+      <c r="AD28">
+        <v>8.9</v>
+      </c>
+      <c r="AE28">
+        <v>2408</v>
+      </c>
+      <c r="AF28">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="AG28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33">
+      <c r="A29" s="2">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>92</v>
+      </c>
+      <c r="C29">
+        <v>26.9</v>
+      </c>
+      <c r="D29">
+        <v>82</v>
+      </c>
+      <c r="E29">
+        <v>28</v>
+      </c>
+      <c r="F29">
+        <v>40</v>
+      </c>
+      <c r="G29">
+        <v>14</v>
+      </c>
+      <c r="H29">
+        <v>70</v>
+      </c>
+      <c r="I29">
+        <v>0.42699999999999999</v>
+      </c>
+      <c r="J29">
+        <v>234</v>
+      </c>
+      <c r="K29">
+        <v>275</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
+      </c>
+      <c r="M29">
+        <v>11</v>
+      </c>
+      <c r="N29">
+        <v>-0.73</v>
+      </c>
+      <c r="O29">
+        <v>-0.1</v>
+      </c>
+      <c r="P29">
+        <v>6.21</v>
+      </c>
+      <c r="Q29">
+        <v>155</v>
+      </c>
+      <c r="R29">
+        <v>180</v>
+      </c>
+      <c r="S29">
+        <v>67</v>
+      </c>
+      <c r="T29">
+        <v>408</v>
+      </c>
+      <c r="U29">
+        <v>16.420000000000002</v>
+      </c>
+      <c r="V29">
+        <v>82</v>
+      </c>
+      <c r="W29">
+        <v>414</v>
+      </c>
+      <c r="X29">
+        <v>80.19</v>
+      </c>
+      <c r="Y29">
+        <v>12</v>
+      </c>
+      <c r="Z29">
+        <v>14</v>
+      </c>
+      <c r="AA29">
+        <v>15</v>
+      </c>
+      <c r="AB29">
+        <v>15.1</v>
+      </c>
+      <c r="AC29">
+        <v>2295</v>
+      </c>
+      <c r="AD29">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="AE29">
+        <v>2734</v>
+      </c>
+      <c r="AF29">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="AG29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33">
+      <c r="A30" s="2">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30">
+        <v>29.2</v>
+      </c>
+      <c r="D30">
+        <v>82</v>
+      </c>
+      <c r="E30">
+        <v>27</v>
+      </c>
+      <c r="F30">
+        <v>41</v>
+      </c>
+      <c r="G30">
+        <v>14</v>
+      </c>
+      <c r="H30">
+        <v>68</v>
+      </c>
+      <c r="I30">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="J30">
+        <v>223</v>
+      </c>
+      <c r="K30">
+        <v>277</v>
+      </c>
+      <c r="L30">
+        <v>4</v>
+      </c>
+      <c r="M30">
+        <v>6</v>
+      </c>
+      <c r="N30">
+        <v>-0.51</v>
+      </c>
+      <c r="O30">
+        <v>0.18</v>
+      </c>
+      <c r="P30">
+        <v>6.1</v>
+      </c>
+      <c r="Q30">
+        <v>136</v>
+      </c>
+      <c r="R30">
+        <v>180</v>
+      </c>
+      <c r="S30">
+        <v>81</v>
+      </c>
+      <c r="T30">
+        <v>442</v>
+      </c>
+      <c r="U30">
+        <v>18.329999999999998</v>
+      </c>
+      <c r="V30">
+        <v>91</v>
+      </c>
+      <c r="W30">
+        <v>411</v>
+      </c>
+      <c r="X30">
+        <v>77.86</v>
+      </c>
+      <c r="Y30">
+        <v>6</v>
+      </c>
+      <c r="Z30">
+        <v>6</v>
+      </c>
+      <c r="AA30">
+        <v>15.1</v>
+      </c>
+      <c r="AB30">
+        <v>16.2</v>
+      </c>
+      <c r="AC30">
+        <v>2542</v>
+      </c>
+      <c r="AD30">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="AE30">
+        <v>2440</v>
+      </c>
+      <c r="AF30">
+        <v>0.88600000000000001</v>
+      </c>
+      <c r="AG30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33">
+      <c r="A31" s="2">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31">
+        <v>28.8</v>
+      </c>
+      <c r="D31">
+        <v>82</v>
+      </c>
+      <c r="E31">
+        <v>31</v>
+      </c>
+      <c r="F31">
+        <v>46</v>
+      </c>
+      <c r="G31">
+        <v>5</v>
+      </c>
+      <c r="H31">
+        <v>67</v>
+      </c>
+      <c r="I31">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="J31">
+        <v>211</v>
+      </c>
+      <c r="K31">
+        <v>282</v>
+      </c>
+      <c r="L31">
+        <v>5</v>
+      </c>
+      <c r="M31">
+        <v>2</v>
+      </c>
+      <c r="N31">
+        <v>-0.64</v>
+      </c>
+      <c r="O31">
+        <v>0.19</v>
+      </c>
+      <c r="P31">
+        <v>6.01</v>
+      </c>
+      <c r="Q31">
+        <v>140</v>
+      </c>
+      <c r="R31">
+        <v>177</v>
+      </c>
+      <c r="S31">
+        <v>66</v>
+      </c>
+      <c r="T31">
+        <v>400</v>
+      </c>
+      <c r="U31">
+        <v>16.5</v>
+      </c>
+      <c r="V31">
+        <v>92</v>
+      </c>
+      <c r="W31">
+        <v>425</v>
+      </c>
+      <c r="X31">
+        <v>78.349999999999994</v>
+      </c>
+      <c r="Y31">
+        <v>5</v>
+      </c>
+      <c r="Z31">
+        <v>13</v>
+      </c>
+      <c r="AA31">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="AB31">
+        <v>15.3</v>
+      </c>
+      <c r="AC31">
+        <v>2320</v>
+      </c>
+      <c r="AD31">
+        <v>9.1</v>
+      </c>
+      <c r="AE31">
+        <v>2470</v>
+      </c>
+      <c r="AF31">
+        <v>0.88600000000000001</v>
+      </c>
+      <c r="AG31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33">
+      <c r="A32" s="2">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32">
+        <v>27.3</v>
+      </c>
+      <c r="D32">
+        <v>82</v>
+      </c>
+      <c r="E32">
+        <v>22</v>
+      </c>
+      <c r="F32">
+        <v>48</v>
+      </c>
+      <c r="G32">
+        <v>12</v>
+      </c>
+      <c r="H32">
+        <v>56</v>
+      </c>
+      <c r="I32">
+        <v>0.34100000000000003</v>
+      </c>
+      <c r="J32">
+        <v>213</v>
+      </c>
+      <c r="K32">
+        <v>297</v>
+      </c>
+      <c r="L32">
+        <v>1</v>
+      </c>
+      <c r="M32">
+        <v>6</v>
+      </c>
+      <c r="N32">
+        <v>-1.1200000000000001</v>
+      </c>
+      <c r="O32">
+        <v>-0.04</v>
+      </c>
+      <c r="P32">
+        <v>6.22</v>
+      </c>
+      <c r="Q32">
+        <v>145</v>
+      </c>
+      <c r="R32">
+        <v>218</v>
+      </c>
+      <c r="S32">
+        <v>53</v>
+      </c>
+      <c r="T32">
+        <v>376</v>
+      </c>
+      <c r="U32">
+        <v>14.1</v>
+      </c>
+      <c r="V32">
+        <v>65</v>
+      </c>
+      <c r="W32">
+        <v>420</v>
+      </c>
+      <c r="X32">
+        <v>84.52</v>
+      </c>
+      <c r="Y32">
+        <v>15</v>
+      </c>
+      <c r="Z32">
+        <v>14</v>
+      </c>
+      <c r="AA32">
+        <v>15.9</v>
+      </c>
+      <c r="AB32">
+        <v>13.6</v>
+      </c>
+      <c r="AC32">
+        <v>2360</v>
+      </c>
+      <c r="AD32">
+        <v>9</v>
+      </c>
+      <c r="AE32">
+        <v>2673</v>
+      </c>
+      <c r="AF32">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="AG32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:33">
+      <c r="A33" s="2"/>
+      <c r="B33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33">
+        <v>28.3</v>
+      </c>
+      <c r="D33">
+        <v>82</v>
+      </c>
+      <c r="E33">
+        <v>41</v>
+      </c>
+      <c r="F33">
+        <v>32</v>
+      </c>
+      <c r="G33">
+        <v>9</v>
+      </c>
+      <c r="H33">
+        <v>91</v>
+      </c>
+      <c r="I33">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="J33">
+        <v>236</v>
+      </c>
+      <c r="K33">
+        <v>236</v>
+      </c>
+      <c r="P33">
+        <v>5.76</v>
+      </c>
+      <c r="Q33">
+        <v>157</v>
+      </c>
+      <c r="R33">
+        <v>157</v>
+      </c>
+      <c r="S33">
+        <v>70</v>
+      </c>
+      <c r="T33">
+        <v>398</v>
+      </c>
+      <c r="U33">
+        <v>17.579999999999998</v>
+      </c>
+      <c r="V33">
+        <v>70</v>
+      </c>
+      <c r="W33">
+        <v>398</v>
+      </c>
+      <c r="X33">
+        <v>82.42</v>
+      </c>
+      <c r="Y33">
+        <v>9</v>
+      </c>
+      <c r="Z33">
+        <v>9</v>
+      </c>
+      <c r="AA33">
+        <v>14.1</v>
+      </c>
+      <c r="AB33">
+        <v>14.1</v>
+      </c>
+      <c r="AC33">
+        <v>2426</v>
+      </c>
+      <c r="AD33">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="AE33">
+        <v>2427</v>
+      </c>
+      <c r="AF33">
+        <v>0.90300000000000002</v>
+      </c>
+      <c r="AG33">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -10668,7 +13960,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:33">
       <c r="A1" s="1"/>
@@ -13946,7 +17238,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:33">
       <c r="A1" s="1"/>
@@ -17224,7 +20516,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:33">
       <c r="A1" s="1"/>
@@ -20502,7 +23794,7 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:33">
       <c r="A1" s="1"/>
@@ -23780,7 +27072,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:33">
       <c r="A1" s="1"/>
@@ -27058,7 +30350,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:33">
       <c r="A1" s="1"/>
@@ -30336,7 +33628,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:33">
       <c r="A1" s="1"/>
@@ -33614,7 +36906,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:33">
       <c r="A1" s="1"/>

</xml_diff>